<commit_message>
Update plan, start PGAdmin doc
</commit_message>
<xml_diff>
--- a/Database Decisions.xlsx
+++ b/Database Decisions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cewar\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cewar\Documents\GitHub\Final_Project_Team2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42857D9E-0F95-4553-A36C-DA2BAF0D4B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE8D373-88C7-4A3D-89DE-2DFC4F8A228B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36" yWindow="72" windowWidth="11772" windowHeight="12240" xr2:uid="{7FEC0537-18EF-4421-BFF8-94667602822C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7FEC0537-18EF-4421-BFF8-94667602822C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,9 +538,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB20E6F5-9ADC-44A7-AD48-C8BCFD044134}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,7 +621,7 @@
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -685,7 +685,7 @@
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -733,7 +733,7 @@
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -741,7 +741,7 @@
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="3" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>